<commit_message>
iCub3 skin GUI cleanup files for upperarms
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/leftUpperArm_ini_generator iCubV3_0.xlsx
+++ b/app/skinGui/iniGenerators/leftUpperArm_ini_generator iCubV3_0.xlsx
@@ -5872,7 +5872,7 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5981,7 +5981,7 @@
       </c>
       <c r="O3" s="24">
         <f>+RADIANS(O5)</f>
-        <v>2.0943951023931953</v>
+        <v>3.1415926535897931</v>
       </c>
       <c r="P3" s="25">
         <v>100</v>
@@ -6069,7 +6069,7 @@
         <v>-2.0943951023932001</v>
       </c>
       <c r="O5" s="39">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="P5" s="34">
         <v>132</v>
@@ -6151,7 +6151,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="39">
-        <v>200</v>
+        <v>130</v>
       </c>
       <c r="P7" s="34">
         <v>148</v>
@@ -6228,7 +6228,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="39">
-        <v>-50</v>
+        <v>190</v>
       </c>
       <c r="P9" s="34">
         <v>164</v>
@@ -6346,26 +6346,26 @@
         <v>16</v>
       </c>
       <c r="B13" s="14">
-        <f t="shared" ref="B3:B25" si="1">((ROUND($L13/10,0))-1)*4+MOD($L13,10)+((J13-1)*15)+O$11</f>
+        <f t="shared" ref="B13:B20" si="1">((ROUND($L13/10,0))-1)*4+MOD($L13,10)+((J13-1)*15)+O$11</f>
         <v>8</v>
       </c>
       <c r="C13" s="15">
-        <f t="shared" ref="C3:C25" si="2">((+P13*COS($O$3)-Q13*SIN($O$3))*$S$3)+$O$7</f>
-        <v>-0.60254037844379127</v>
+        <f t="shared" ref="C13:C20" si="2">((+P13*COS($O$3)-Q13*SIN($O$3))*$S$3)+$O$7</f>
+        <v>-2.0000000000000284</v>
       </c>
       <c r="D13" s="15">
-        <f t="shared" ref="D3:D20" si="3">((P13*SIN($O$3)+Q13*COS($O$3))*$S$4)+$O$9</f>
-        <v>-13.397459621556067</v>
+        <f t="shared" ref="D13:D20" si="3">((P13*SIN($O$3)+Q13*COS($O$3))*$S$4)+$O$9</f>
+        <v>34.574374157796029</v>
       </c>
       <c r="E13" s="15">
-        <f t="shared" ref="E3:E13" si="4">S$3*(($N13/3.1416*180)+$O$5)</f>
-        <v>120</v>
+        <f t="shared" ref="E13" si="4">S$3*(($N13/3.1416*180)+$O$5)</f>
+        <v>180</v>
       </c>
       <c r="F13" s="16">
         <v>4</v>
       </c>
       <c r="G13" s="17">
-        <f t="shared" ref="G3:G25" si="5">IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" ref="G13:G20" si="5">IF($S$3*$S$4=-1,1,0)</f>
         <v>0</v>
       </c>
       <c r="I13" s="18"/>
@@ -6403,15 +6403,15 @@
       </c>
       <c r="C14" s="15">
         <f t="shared" si="2"/>
-        <v>-0.60254037844376285</v>
+        <v>13.999999999999986</v>
       </c>
       <c r="D14" s="15">
         <f t="shared" si="3"/>
-        <v>-31.872668235624062</v>
+        <v>25.336769850762039</v>
       </c>
       <c r="E14" s="15">
         <f>S$3*(($N14/3.1416*180)+$O$5)</f>
-        <v>179.99985969422843</v>
+        <v>239.99985969422843</v>
       </c>
       <c r="F14" s="16">
         <v>4</v>
@@ -6455,15 +6455,15 @@
       </c>
       <c r="C15" s="15">
         <f t="shared" si="2"/>
-        <v>-16.602540378443763</v>
+        <v>13.999999999999972</v>
       </c>
       <c r="D15" s="15">
         <f t="shared" si="3"/>
-        <v>-41.110272542658066</v>
+        <v>6.8615612366940013</v>
       </c>
       <c r="E15" s="15">
         <f t="shared" ref="E15:E20" si="6">S$3*(($N15/3.1416*180)+$O$5)</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F15" s="16">
         <v>4</v>
@@ -6507,15 +6507,15 @@
       </c>
       <c r="C16" s="15">
         <f t="shared" si="2"/>
-        <v>-32.602540378443734</v>
+        <v>-2.0000000000000284</v>
       </c>
       <c r="D16" s="15">
         <f t="shared" si="3"/>
-        <v>-31.872668235624047</v>
+        <v>-2.3760430703399607</v>
       </c>
       <c r="E16" s="15">
         <f t="shared" si="6"/>
-        <v>60.000140305771573</v>
+        <v>120.00014030577157</v>
       </c>
       <c r="F16" s="16">
         <v>4</v>
@@ -6559,15 +6559,15 @@
       </c>
       <c r="C17" s="15">
         <f t="shared" si="2"/>
-        <v>-16.602540378443734</v>
+        <v>29.999999999999972</v>
       </c>
       <c r="D17" s="15">
         <f t="shared" si="3"/>
-        <v>-59.585481156726075</v>
+        <v>-2.3760430703399891</v>
       </c>
       <c r="E17" s="15">
         <f t="shared" si="6"/>
-        <v>179.99985969422843</v>
+        <v>239.99985969422843</v>
       </c>
       <c r="F17" s="16">
         <v>4</v>
@@ -6611,15 +6611,15 @@
       </c>
       <c r="C18" s="15">
         <f t="shared" si="2"/>
-        <v>-0.60254037844376285</v>
+        <v>45.999999999999972</v>
       </c>
       <c r="D18" s="15">
         <f t="shared" si="3"/>
-        <v>-68.823085463760108</v>
+        <v>6.8615612366940013</v>
       </c>
       <c r="E18" s="15">
         <f t="shared" si="6"/>
-        <v>239.99971938845687</v>
+        <v>299.99971938845687</v>
       </c>
       <c r="F18" s="16">
         <v>4</v>
@@ -6663,15 +6663,15 @@
       </c>
       <c r="C19" s="15">
         <f t="shared" si="2"/>
-        <v>15.397459621556209</v>
+        <v>29.999999999999986</v>
       </c>
       <c r="D19" s="15">
         <f t="shared" si="3"/>
-        <v>-41.110272542658095</v>
+        <v>34.574374157796001</v>
       </c>
       <c r="E19" s="15">
         <f t="shared" si="6"/>
-        <v>239.99971938845687</v>
+        <v>299.99971938845687</v>
       </c>
       <c r="F19" s="16">
         <v>4</v>
@@ -6715,15 +6715,15 @@
       </c>
       <c r="C20" s="15">
         <f t="shared" si="2"/>
-        <v>15.397459621556237</v>
+        <v>45.999999999999986</v>
       </c>
       <c r="D20" s="15">
         <f t="shared" si="3"/>
-        <v>-59.585481156726104</v>
+        <v>25.33676985076201</v>
       </c>
       <c r="E20" s="15">
         <f t="shared" si="6"/>
-        <v>179.99985969422843</v>
+        <v>239.99985969422843</v>
       </c>
       <c r="F20" s="16">
         <v>4</v>
@@ -7297,19 +7297,19 @@
         <v>16</v>
       </c>
       <c r="B3" s="14">
-        <f t="shared" ref="B3:B20" si="0">((ROUND($L3/10,0))-1)*4+MOD($L3,10)+((J3-1)*15)+O$11</f>
+        <f t="shared" ref="B3:B12" si="0">((ROUND($L3/10,0))-1)*4+MOD($L3,10)+((J3-1)*15)+O$11</f>
         <v>0</v>
       </c>
       <c r="C3" s="15">
-        <f t="shared" ref="C3:C20" si="1">((+P3*COS($O$3)-Q3*SIN($O$3))*$S$3)+$O$7</f>
+        <f t="shared" ref="C3:C12" si="1">((+P3*COS($O$3)-Q3*SIN($O$3))*$S$3)+$O$7</f>
         <v>136.60254037844388</v>
       </c>
       <c r="D3" s="15">
-        <f t="shared" ref="D3:D20" si="2">((P3*SIN($O$3)+Q3*COS($O$3))*$S$4)+$O$9</f>
+        <f t="shared" ref="D3:D12" si="2">((P3*SIN($O$3)+Q3*COS($O$3))*$S$4)+$O$9</f>
         <v>-36.602540378443848</v>
       </c>
       <c r="E3" s="15">
-        <f t="shared" ref="E3:E13" si="3">S$3*(($N3/3.1416*180)+$O$5)</f>
+        <f t="shared" ref="E3:E12" si="3">S$3*(($N3/3.1416*180)+$O$5)</f>
         <v>180.00028061154313</v>
       </c>
       <c r="F3" s="16">
@@ -8550,7 +8550,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+      <selection activeCell="A13" sqref="A13:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8890,15 +8890,15 @@
       </c>
       <c r="C13" s="56">
         <f>IF('left upperarm front'!C13=0, "", 'left upperarm front'!C13)</f>
-        <v>-0.60254037844379127</v>
+        <v>-2.0000000000000284</v>
       </c>
       <c r="D13" s="56">
         <f>IF('left upperarm front'!D13=0, "", 'left upperarm front'!D13)</f>
-        <v>-13.397459621556067</v>
+        <v>34.574374157796029</v>
       </c>
       <c r="E13" s="56">
         <f>IF('left upperarm front'!E13=0, "", 'left upperarm front'!E13)</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F13" s="56">
         <f>IF('left upperarm front'!F13=0, "", 'left upperarm front'!F13)</f>
@@ -8920,15 +8920,15 @@
       </c>
       <c r="C14" s="56">
         <f>IF('left upperarm front'!C14=0, "", 'left upperarm front'!C14)</f>
-        <v>-0.60254037844376285</v>
+        <v>13.999999999999986</v>
       </c>
       <c r="D14" s="56">
         <f>IF('left upperarm front'!D14=0, "", 'left upperarm front'!D14)</f>
-        <v>-31.872668235624062</v>
+        <v>25.336769850762039</v>
       </c>
       <c r="E14" s="56">
         <f>IF('left upperarm front'!E14=0, "", 'left upperarm front'!E14)</f>
-        <v>179.99985969422843</v>
+        <v>239.99985969422843</v>
       </c>
       <c r="F14" s="56">
         <f>IF('left upperarm front'!F14=0, "", 'left upperarm front'!F14)</f>
@@ -8950,15 +8950,15 @@
       </c>
       <c r="C15" s="56">
         <f>IF('left upperarm front'!C15=0, "", 'left upperarm front'!C15)</f>
-        <v>-16.602540378443763</v>
+        <v>13.999999999999972</v>
       </c>
       <c r="D15" s="56">
         <f>IF('left upperarm front'!D15=0, "", 'left upperarm front'!D15)</f>
-        <v>-41.110272542658066</v>
+        <v>6.8615612366940013</v>
       </c>
       <c r="E15" s="56">
         <f>IF('left upperarm front'!E15=0, "", 'left upperarm front'!E15)</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F15" s="56">
         <f>IF('left upperarm front'!F15=0, "", 'left upperarm front'!F15)</f>
@@ -8980,15 +8980,15 @@
       </c>
       <c r="C16" s="56">
         <f>IF('left upperarm front'!C16=0, "", 'left upperarm front'!C16)</f>
-        <v>-32.602540378443734</v>
+        <v>-2.0000000000000284</v>
       </c>
       <c r="D16" s="56">
         <f>IF('left upperarm front'!D16=0, "", 'left upperarm front'!D16)</f>
-        <v>-31.872668235624047</v>
+        <v>-2.3760430703399607</v>
       </c>
       <c r="E16" s="56">
         <f>IF('left upperarm front'!E16=0, "", 'left upperarm front'!E16)</f>
-        <v>60.000140305771573</v>
+        <v>120.00014030577157</v>
       </c>
       <c r="F16" s="56">
         <f>IF('left upperarm front'!F16=0, "", 'left upperarm front'!F16)</f>
@@ -9010,15 +9010,15 @@
       </c>
       <c r="C17" s="56">
         <f>IF('left upperarm front'!C17=0, "", 'left upperarm front'!C17)</f>
-        <v>-16.602540378443734</v>
+        <v>29.999999999999972</v>
       </c>
       <c r="D17" s="56">
         <f>IF('left upperarm front'!D17=0, "", 'left upperarm front'!D17)</f>
-        <v>-59.585481156726075</v>
+        <v>-2.3760430703399891</v>
       </c>
       <c r="E17" s="56">
         <f>IF('left upperarm front'!E17=0, "", 'left upperarm front'!E17)</f>
-        <v>179.99985969422843</v>
+        <v>239.99985969422843</v>
       </c>
       <c r="F17" s="56">
         <f>IF('left upperarm front'!F17=0, "", 'left upperarm front'!F17)</f>
@@ -9040,15 +9040,15 @@
       </c>
       <c r="C18" s="56">
         <f>IF('left upperarm front'!C18=0, "", 'left upperarm front'!C18)</f>
-        <v>-0.60254037844376285</v>
+        <v>45.999999999999972</v>
       </c>
       <c r="D18" s="56">
         <f>IF('left upperarm front'!D18=0, "", 'left upperarm front'!D18)</f>
-        <v>-68.823085463760108</v>
+        <v>6.8615612366940013</v>
       </c>
       <c r="E18" s="56">
         <f>IF('left upperarm front'!E18=0, "", 'left upperarm front'!E18)</f>
-        <v>239.99971938845687</v>
+        <v>299.99971938845687</v>
       </c>
       <c r="F18" s="56">
         <f>IF('left upperarm front'!F18=0, "", 'left upperarm front'!F18)</f>
@@ -9070,15 +9070,15 @@
       </c>
       <c r="C19" s="56">
         <f>IF('left upperarm front'!C19=0, "", 'left upperarm front'!C19)</f>
-        <v>15.397459621556209</v>
+        <v>29.999999999999986</v>
       </c>
       <c r="D19" s="56">
         <f>IF('left upperarm front'!D19=0, "", 'left upperarm front'!D19)</f>
-        <v>-41.110272542658095</v>
+        <v>34.574374157796001</v>
       </c>
       <c r="E19" s="56">
         <f>IF('left upperarm front'!E19=0, "", 'left upperarm front'!E19)</f>
-        <v>239.99971938845687</v>
+        <v>299.99971938845687</v>
       </c>
       <c r="F19" s="56">
         <f>IF('left upperarm front'!F19=0, "", 'left upperarm front'!F19)</f>
@@ -9100,15 +9100,15 @@
       </c>
       <c r="C20" s="56">
         <f>IF('left upperarm front'!C20=0, "", 'left upperarm front'!C20)</f>
-        <v>15.397459621556237</v>
+        <v>45.999999999999986</v>
       </c>
       <c r="D20" s="56">
         <f>IF('left upperarm front'!D20=0, "", 'left upperarm front'!D20)</f>
-        <v>-59.585481156726104</v>
+        <v>25.33676985076201</v>
       </c>
       <c r="E20" s="56">
         <f>IF('left upperarm front'!E20=0, "", 'left upperarm front'!E20)</f>
-        <v>179.99985969422843</v>
+        <v>239.99985969422843</v>
       </c>
       <c r="F20" s="56">
         <f>IF('left upperarm front'!F20=0, "", 'left upperarm front'!F20)</f>

</xml_diff>